<commit_message>
feat: Completar práctica de clustering.
</commit_message>
<xml_diff>
--- a/2022/Practica 1 - Clustering/estaturas.xlsx
+++ b/2022/Practica 1 - Clustering/estaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dany\Documents\01 Dany\Maestría\3er trimestre\Statistical Learning II\Practicas\Practica 1 - Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E29E5-1ACB-4185-85EF-09107801EB81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A095D2AF-1FED-4273-9800-99938D0ED727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t>Estatura(metros)</t>
   </si>
@@ -173,14 +173,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,8 +400,8 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -827,8 +826,8 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="6">
-        <v>1.68</v>
+      <c r="A53" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B53" s="4">
         <v>34</v>

</xml_diff>